<commit_message>
Lille ændring i tidsregistrering (Alexander)
</commit_message>
<xml_diff>
--- a/08-Project-Management/Tidsregistrering/Tidsregistrering (Alexander).xlsx
+++ b/08-Project-Management/Tidsregistrering/Tidsregistrering (Alexander).xlsx
@@ -382,7 +382,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -393,7 +393,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -459,7 +459,7 @@
         <v>42059</v>
       </c>
       <c r="B5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
AD, DOM og testcases for UC-3
</commit_message>
<xml_diff>
--- a/08-Project-Management/Tidsregistrering/Tidsregistrering (Alexander).xlsx
+++ b/08-Project-Management/Tidsregistrering/Tidsregistrering (Alexander).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Navn</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>Test case writing</t>
+  </si>
+  <si>
+    <t>Aktivitetsdiagram, domænemodel</t>
+  </si>
+  <si>
+    <t>Test case implementation</t>
+  </si>
+  <si>
+    <t>Test Designer</t>
   </si>
 </sst>
 </file>
@@ -408,7 +417,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -541,22 +550,64 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="4">
-        <v>42060</v>
+        <v>42061</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="4">
-        <v>42060</v>
+        <v>42061</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12"/>
+      <c r="A12" s="4">
+        <v>42062</v>
+      </c>
+      <c r="B12">
+        <v>2.5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13"/>
+      <c r="A13" s="4">
+        <v>42062</v>
+      </c>
+      <c r="B13">
+        <v>0.5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14"/>
+      <c r="A14" s="4">
+        <v>42062</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15"/>

</xml_diff>